<commit_message>
assignment 2 and special assignment
</commit_message>
<xml_diff>
--- a/Contents.xlsx
+++ b/Contents.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Banu\Medusind\M_B1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A01F71-6FE8-498F-A940-7918BE4E160C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DC9304-F58E-4250-A050-ED109099E063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{65638B01-F78A-4D79-B924-A215ED419263}"/>
   </bookViews>
@@ -879,7 +879,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -890,7 +890,7 @@
   <dimension ref="B2:C107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1016,7 @@
       <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="18" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1040,7 +1040,7 @@
       <c r="B20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="18" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
       <c r="B21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="18" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Day5 Csharp + Assignment 4
</commit_message>
<xml_diff>
--- a/Contents.xlsx
+++ b/Contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Banu\Medusind\M_B1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33904499-CDA5-43A9-9BF1-C619E4D20679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1079BF65-9EE2-48D9-B73D-D36F310E5D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{65638B01-F78A-4D79-B924-A215ED419263}"/>
   </bookViews>
@@ -521,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -577,6 +577,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -895,8 +898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1085E8FD-83CE-480C-BA28-A761F4AEF31A}">
   <dimension ref="B2:C107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,19 +1125,19 @@
       <c r="C30" s="1"/>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="19" t="s">
         <v>48</v>
       </c>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="19" t="s">
         <v>49</v>
       </c>
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="19" t="s">
         <v>50</v>
       </c>
       <c r="C33" s="1"/>
@@ -1146,7 +1149,7 @@
       <c r="C34" s="1"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="19" t="s">
         <v>52</v>
       </c>
       <c r="C35" s="1"/>
@@ -1168,13 +1171,13 @@
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="21" t="s">
         <v>54</v>
       </c>
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="21" t="s">
         <v>55</v>
       </c>
       <c r="C40" s="1"/>

</xml_diff>

<commit_message>
MVC helpers n Validations
</commit_message>
<xml_diff>
--- a/Contents.xlsx
+++ b/Contents.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Banu\Medusind\M_B1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F44A3B0-6A1B-4889-9084-6867EC0B76ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E406132-C479-44B1-8F39-A813892E9526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{65638B01-F78A-4D79-B924-A215ED419263}"/>
   </bookViews>
@@ -521,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -543,9 +543,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -895,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1085E8FD-83CE-480C-BA28-A761F4AEF31A}">
   <dimension ref="B2:C107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,50 +915,50 @@
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>11</v>
       </c>
     </row>
@@ -969,12 +966,12 @@
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>14</v>
       </c>
     </row>
@@ -982,177 +979,177 @@
       <c r="B12" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C28" s="1"/>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>47</v>
       </c>
       <c r="C30" s="1"/>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>50</v>
       </c>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="14" t="s">
         <v>51</v>
       </c>
       <c r="C34" s="1"/>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="14" t="s">
         <v>52</v>
       </c>
       <c r="C35" s="1"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="14" t="s">
         <v>53</v>
       </c>
       <c r="C36" s="1"/>
@@ -1168,19 +1165,19 @@
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="16" t="s">
         <v>54</v>
       </c>
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="16" t="s">
         <v>55</v>
       </c>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="16" t="s">
         <v>56</v>
       </c>
       <c r="C41" s="1"/>
@@ -1196,31 +1193,31 @@
       <c r="C43" s="1"/>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="17" t="s">
         <v>57</v>
       </c>
       <c r="C44" s="1"/>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="18" t="s">
+      <c r="B45" s="17" t="s">
         <v>58</v>
       </c>
       <c r="C45" s="1"/>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="18" t="s">
+      <c r="B46" s="17" t="s">
         <v>59</v>
       </c>
       <c r="C46" s="1"/>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="19" t="s">
+      <c r="B47" s="18" t="s">
         <v>107</v>
       </c>
       <c r="C47" s="1"/>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="17" t="s">
         <v>102</v>
       </c>
       <c r="C48" s="1"/>
@@ -1236,37 +1233,37 @@
       <c r="C50" s="1"/>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="17" t="s">
         <v>60</v>
       </c>
       <c r="C51" s="1"/>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="18" t="s">
+      <c r="B52" s="17" t="s">
         <v>61</v>
       </c>
       <c r="C52" s="1"/>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="18" t="s">
+      <c r="B53" s="17" t="s">
         <v>62</v>
       </c>
       <c r="C53" s="1"/>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B54" s="18" t="s">
+      <c r="B54" s="17" t="s">
         <v>118</v>
       </c>
       <c r="C54" s="1"/>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B55" s="18" t="s">
+      <c r="B55" s="17" t="s">
         <v>63</v>
       </c>
       <c r="C55" s="1"/>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="16" t="s">
+      <c r="B56" s="15" t="s">
         <v>64</v>
       </c>
       <c r="C56" s="1"/>
@@ -1286,55 +1283,55 @@
       <c r="C59" s="1"/>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="19" t="s">
         <v>65</v>
       </c>
       <c r="C60" s="1"/>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="19" t="s">
         <v>66</v>
       </c>
       <c r="C61" s="1"/>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="19" t="s">
         <v>67</v>
       </c>
       <c r="C62" s="1"/>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B63" s="20" t="s">
+      <c r="B63" s="19" t="s">
         <v>68</v>
       </c>
       <c r="C63" s="1"/>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="20" t="s">
+      <c r="B64" s="19" t="s">
         <v>69</v>
       </c>
       <c r="C64" s="1"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="20" t="s">
+      <c r="B65" s="19" t="s">
         <v>70</v>
       </c>
       <c r="C65" s="1"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="20" t="s">
+      <c r="B66" s="19" t="s">
         <v>71</v>
       </c>
       <c r="C66" s="1"/>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="19" t="s">
         <v>72</v>
       </c>
       <c r="C67" s="1"/>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="19" t="s">
         <v>73</v>
       </c>
       <c r="C68" s="1"/>
@@ -1354,61 +1351,61 @@
       <c r="C71" s="1"/>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="16" t="s">
+      <c r="B72" s="15" t="s">
         <v>74</v>
       </c>
       <c r="C72" s="1"/>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="16" t="s">
+      <c r="B73" s="15" t="s">
         <v>75</v>
       </c>
       <c r="C73" s="1"/>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="16" t="s">
+      <c r="B74" s="15" t="s">
         <v>76</v>
       </c>
       <c r="C74" s="1"/>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="16" t="s">
+      <c r="B75" s="15" t="s">
         <v>77</v>
       </c>
       <c r="C75" s="1"/>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="16" t="s">
+      <c r="B76" s="15" t="s">
         <v>78</v>
       </c>
       <c r="C76" s="1"/>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="15" t="s">
         <v>79</v>
       </c>
       <c r="C77" s="1"/>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="16" t="s">
+      <c r="B78" s="15" t="s">
         <v>80</v>
       </c>
       <c r="C78" s="1"/>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="8" t="s">
+      <c r="B79" s="16" t="s">
         <v>81</v>
       </c>
       <c r="C79" s="1"/>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="15" t="s">
         <v>82</v>
       </c>
       <c r="C80" s="1"/>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="16" t="s">
+      <c r="B81" s="15" t="s">
         <v>83</v>
       </c>
       <c r="C81" s="1"/>
@@ -1426,13 +1423,13 @@
       <c r="C83" s="1"/>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="16" t="s">
+      <c r="B84" s="15" t="s">
         <v>86</v>
       </c>
       <c r="C84" s="1"/>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B85" s="10" t="s">
+      <c r="B85" s="9" t="s">
         <v>103</v>
       </c>
       <c r="C85" s="1"/>
@@ -1448,56 +1445,56 @@
       <c r="C87" s="1"/>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="12" t="s">
+      <c r="B88" s="11" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" s="13" t="s">
+      <c r="B89" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B90" s="13" t="s">
+      <c r="B90" s="12" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B91" s="13" t="s">
+      <c r="B91" s="12" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B92" s="13" t="s">
+      <c r="B92" s="12" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B93" s="13" t="s">
+      <c r="B93" s="12" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="13" t="s">
+      <c r="B94" s="12" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="13" t="s">
+      <c r="B95" s="12" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B96" s="13" t="s">
+      <c r="B96" s="12" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="10"/>
+      <c r="B97" s="9"/>
       <c r="C97" s="1"/>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="11" t="s">
+      <c r="B98" s="10" t="s">
         <v>117</v>
       </c>
       <c r="C98" s="1"/>

</xml_diff>